<commit_message>
added read and write excel file method
</commit_message>
<xml_diff>
--- a/BackendAPIOutsmart/src/test/resources/TestDataOutsmart.xlsx
+++ b/BackendAPIOutsmart/src/test/resources/TestDataOutsmart.xlsx
@@ -12,7 +12,7 @@
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -58,6 +58,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -442,31 +443,31 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="0">
         <v>7676565456</v>
       </c>
       <c r="D2" s="1" t="s">

</xml_diff>